<commit_message>
Updated excel file for scenario 1
Updated excel file for scenario 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MasterTestData.xlsx
+++ b/src/test/resources/TestData/MasterTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pravesh.jha\Desktop\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SVN_Pravesh_Repository\GIT_LovesCloud\projecttest\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,25 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>Calibrate TV Channel-Prepopulating configured values</t>
-  </si>
-  <si>
-    <t>Add Channel to the Plan with Values selected for TV,Video on Demand and Online Videos</t>
-  </si>
-  <si>
-    <t>CPM is uneditable for Channels youtube(Auction),facebook and Instagram</t>
-  </si>
-  <si>
-    <t>CPM is editable for Channel youtube(Reservation,GooglePreferred)</t>
-  </si>
-  <si>
-    <t>Overwriting CPM for Channels TV,VideoOnDemand and Online+Video and Saving for Plan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>buyingAudience</t>
   </si>
@@ -53,13 +35,64 @@
   </si>
   <si>
     <t>Comparison setup page - Edit Scenarios</t>
+  </si>
+  <si>
+    <t>ScenarioID</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ChannelNameTV</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>TVbuyingAudience</t>
+  </si>
+  <si>
+    <t>TVDONOTDELETE</t>
+  </si>
+  <si>
+    <t>TVSecondLengthFormat</t>
+  </si>
+  <si>
+    <t>DefaultCPMforTV</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>DefaultGRPs</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>DefaultReach</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>DefaultMaximumReach</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>DefaultPrecision</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +113,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -103,7 +149,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -163,11 +209,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -185,11 +242,250 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -274,43 +570,43 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -516,20 +812,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <tableColumns count="2">
-    <tableColumn id="1" name="Scenario" dataDxfId="8"/>
-    <tableColumn id="2" name="buyingAudience" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <tableColumns count="9">
+    <tableColumn id="1" name="ScenarioID" dataDxfId="15"/>
+    <tableColumn id="2" name="ChannelNameTV" dataDxfId="14"/>
+    <tableColumn id="3" name="TVbuyingAudience" dataDxfId="6"/>
+    <tableColumn id="5" name="TVSecondLengthFormat" dataDxfId="5"/>
+    <tableColumn id="6" name="DefaultCPMforTV" dataDxfId="4"/>
+    <tableColumn id="7" name="DefaultGRPs" dataDxfId="3"/>
+    <tableColumn id="8" name="DefaultReach" dataDxfId="2"/>
+    <tableColumn id="9" name="DefaultMaximumReach" dataDxfId="1"/>
+    <tableColumn id="10" name="DefaultPrecision" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:B4" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <tableColumns count="2">
-    <tableColumn id="1" name="Scenario" dataDxfId="1"/>
-    <tableColumn id="2" name="buyingAudience" dataDxfId="0"/>
+    <tableColumn id="1" name="ScenarioID" dataDxfId="8"/>
+    <tableColumn id="2" name="buyingAudience" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -825,57 +1128,83 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" spans="1:2" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" spans="1:2" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" spans="1:2" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -895,7 +1224,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,27 +1236,27 @@
   <sheetData>
     <row r="1" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" s="4" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5"/>
     </row>

</xml_diff>

<commit_message>
Test Data Implementioan for scenario 1
Test Data Implementioan for scenario 1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MasterTestData.xlsx
+++ b/src/test/resources/TestData/MasterTestData.xlsx
@@ -61,9 +61,6 @@
     <t>DefaultCPMforTV</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>DefaultGRPs</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>20.00</t>
   </si>
 </sst>
 </file>
@@ -261,6 +261,162 @@
   <dxfs count="21">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -484,162 +640,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -816,23 +816,23 @@
   <tableColumns count="9">
     <tableColumn id="1" name="ScenarioID" dataDxfId="15"/>
     <tableColumn id="2" name="ChannelNameTV" dataDxfId="14"/>
-    <tableColumn id="3" name="TVbuyingAudience" dataDxfId="6"/>
-    <tableColumn id="5" name="TVSecondLengthFormat" dataDxfId="5"/>
-    <tableColumn id="6" name="DefaultCPMforTV" dataDxfId="4"/>
-    <tableColumn id="7" name="DefaultGRPs" dataDxfId="3"/>
-    <tableColumn id="8" name="DefaultReach" dataDxfId="2"/>
-    <tableColumn id="9" name="DefaultMaximumReach" dataDxfId="1"/>
-    <tableColumn id="10" name="DefaultPrecision" dataDxfId="0"/>
+    <tableColumn id="3" name="TVbuyingAudience" dataDxfId="13"/>
+    <tableColumn id="5" name="TVSecondLengthFormat" dataDxfId="12"/>
+    <tableColumn id="6" name="DefaultCPMforTV" dataDxfId="11"/>
+    <tableColumn id="7" name="DefaultGRPs" dataDxfId="10"/>
+    <tableColumn id="8" name="DefaultReach" dataDxfId="9"/>
+    <tableColumn id="9" name="DefaultMaximumReach" dataDxfId="8"/>
+    <tableColumn id="10" name="DefaultPrecision" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:B4" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="A1:B4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <tableColumns count="2">
-    <tableColumn id="1" name="ScenarioID" dataDxfId="8"/>
-    <tableColumn id="2" name="buyingAudience" dataDxfId="7"/>
+    <tableColumn id="1" name="ScenarioID" dataDxfId="1"/>
+    <tableColumn id="2" name="buyingAudience" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,7 +1132,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,16 +1165,16 @@
         <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,19 +1191,19 @@
         <v>9</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated as per rajni suggestion
Updated as per rajni suggestion
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MasterTestData.xlsx
+++ b/src/test/resources/TestData/MasterTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>buyingAudience</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>ChannelNameTV</t>
-  </si>
-  <si>
-    <t>TV</t>
   </si>
   <si>
     <t>TVbuyingAudience</t>
@@ -258,7 +252,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="20">
     <dxf>
       <font>
         <b val="0"/>
@@ -640,44 +634,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -812,10 +768,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:I2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="16">
-  <tableColumns count="9">
-    <tableColumn id="1" name="ScenarioID" dataDxfId="15"/>
-    <tableColumn id="2" name="ChannelNameTV" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <tableColumns count="8">
+    <tableColumn id="1" name="ScenarioID" dataDxfId="14"/>
     <tableColumn id="3" name="TVbuyingAudience" dataDxfId="13"/>
     <tableColumn id="5" name="TVSecondLengthFormat" dataDxfId="12"/>
     <tableColumn id="6" name="DefaultCPMforTV" dataDxfId="11"/>
@@ -1128,41 +1083,40 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="15.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="11.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>12</v>
@@ -1173,27 +1127,24 @@
       <c r="H1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
@@ -1201,9 +1152,6 @@
       </c>
       <c r="H2" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
before code added for
before code added for
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/MasterTestData.xlsx
+++ b/src/test/resources/TestData/MasterTestData.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7620" tabRatio="647"/>
   </bookViews>
   <sheets>
-    <sheet name="Channel selection" sheetId="21" r:id="rId1"/>
+    <sheet name="channel_selection" sheetId="21" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="GMT_12_00__International_Date_Line_West">#REF!</definedName>
@@ -545,7 +545,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>